<commit_message>
Update custom DB tools
</commit_message>
<xml_diff>
--- a/customDBtools/customDBs.xlsx
+++ b/customDBtools/customDBs.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="18120" windowHeight="4050" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="18120" windowHeight="4050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dakar raw" sheetId="1" r:id="rId1"/>
     <sheet name="Dakar" sheetId="2" r:id="rId2"/>
     <sheet name="HardEnduro raw" sheetId="3" r:id="rId3"/>
     <sheet name="HardEnduro" sheetId="4" r:id="rId4"/>
+    <sheet name="SuperEnduro raw" sheetId="5" r:id="rId5"/>
+    <sheet name="SuperEnduro" sheetId="6" r:id="rId6"/>
+    <sheet name="NOTES" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
   <si>
     <t xml:space="preserve"> Start podium in Buenos Aires / Prologue / Liaison to Bivouac "0" close to Rosario</t>
   </si>
@@ -182,12 +185,86 @@
   </si>
   <si>
     <t>Red Bull Hard Enduro</t>
+  </si>
+  <si>
+    <t>GP Poland</t>
+  </si>
+  <si>
+    <t>Lodz/Atlas Arena</t>
+  </si>
+  <si>
+    <t>GP Germany</t>
+  </si>
+  <si>
+    <t>Riesa/SachsenArena</t>
+  </si>
+  <si>
+    <t>GP Italy</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>GP AMV Argentina</t>
+  </si>
+  <si>
+    <t>Pinamar</t>
+  </si>
+  <si>
+    <t>GP Brazil</t>
+  </si>
+  <si>
+    <t>Belo Horizonte/Mineirinho</t>
+  </si>
+  <si>
+    <t>GP Czech Republic</t>
+  </si>
+  <si>
+    <t>Prague/Tipsport Arena</t>
+  </si>
+  <si>
+    <t>SuperEnduro</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Lodz</t>
+  </si>
+  <si>
+    <t>Riesa</t>
+  </si>
+  <si>
+    <t>Belo Horizonte</t>
+  </si>
+  <si>
+    <t>Prague</t>
+  </si>
+  <si>
+    <t>Export sheet as CSV</t>
+  </si>
+  <si>
+    <t>Used below to convert CSV to JSON
+http://codebeautify.org/csv-to-xml-json
+http://www.convertcsv.com/csv-to-json.htm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -666,10 +743,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1154,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1862,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,4 +2318,440 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3">
+        <v>42343</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42371</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42385</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3">
+        <v>42420</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3">
+        <v>42427</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3">
+        <v>42441</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="38.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>999902</v>
+      </c>
+      <c r="B2" s="4">
+        <f>'SuperEnduro raw'!B1</f>
+        <v>42343</v>
+      </c>
+      <c r="C2">
+        <v>2016</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="str">
+        <f>'SuperEnduro raw'!C1</f>
+        <v>GP Poland</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>'SuperEnduro raw'!D1</f>
+        <v>Lodz/Atlas Arena</v>
+      </c>
+      <c r="H2" t="str">
+        <f>'SuperEnduro raw'!A1</f>
+        <v>Poland</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="str">
+        <f>CONCATENATE(H2, " - ",G2)</f>
+        <v>Poland - Lodz/Atlas Arena</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>999902</v>
+      </c>
+      <c r="B3" s="4">
+        <f>'SuperEnduro raw'!B2</f>
+        <v>42371</v>
+      </c>
+      <c r="C3">
+        <v>2016</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="str">
+        <f>'SuperEnduro raw'!C2</f>
+        <v>GP Germany</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="str">
+        <f>'SuperEnduro raw'!D2</f>
+        <v>Riesa/SachsenArena</v>
+      </c>
+      <c r="H3" t="str">
+        <f>'SuperEnduro raw'!A2</f>
+        <v>Germany</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J7" si="0">CONCATENATE(H3, " - ",G3)</f>
+        <v>Germany - Riesa/SachsenArena</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>999902</v>
+      </c>
+      <c r="B4" s="4">
+        <f>'SuperEnduro raw'!B3</f>
+        <v>42385</v>
+      </c>
+      <c r="C4">
+        <v>2016</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="str">
+        <f>'SuperEnduro raw'!C3</f>
+        <v>GP Italy</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f>'SuperEnduro raw'!D3</f>
+        <v>Cancel</v>
+      </c>
+      <c r="H4" t="str">
+        <f>'SuperEnduro raw'!A3</f>
+        <v>Italy</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Italy - Cancel</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>999902</v>
+      </c>
+      <c r="B5" s="4">
+        <f>'SuperEnduro raw'!B4</f>
+        <v>42420</v>
+      </c>
+      <c r="C5">
+        <v>2016</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="str">
+        <f>'SuperEnduro raw'!C4</f>
+        <v>GP AMV Argentina</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="str">
+        <f>'SuperEnduro raw'!D4</f>
+        <v>Pinamar</v>
+      </c>
+      <c r="H5" t="str">
+        <f>'SuperEnduro raw'!A4</f>
+        <v>Argentina</v>
+      </c>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Argentina - Pinamar</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>999902</v>
+      </c>
+      <c r="B6" s="4">
+        <f>'SuperEnduro raw'!B5</f>
+        <v>42427</v>
+      </c>
+      <c r="C6">
+        <v>2016</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="str">
+        <f>'SuperEnduro raw'!C5</f>
+        <v>GP Brazil</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="str">
+        <f>'SuperEnduro raw'!D5</f>
+        <v>Belo Horizonte/Mineirinho</v>
+      </c>
+      <c r="H6" t="str">
+        <f>'SuperEnduro raw'!A5</f>
+        <v>Brazil</v>
+      </c>
+      <c r="I6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Brazil - Belo Horizonte/Mineirinho</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>999902</v>
+      </c>
+      <c r="B7" s="4">
+        <f>'SuperEnduro raw'!B6</f>
+        <v>42441</v>
+      </c>
+      <c r="C7">
+        <v>2016</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="str">
+        <f>'SuperEnduro raw'!C6</f>
+        <v>GP Czech Republic</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="str">
+        <f>'SuperEnduro raw'!D6</f>
+        <v>Prague/Tipsport Arena</v>
+      </c>
+      <c r="H7" t="str">
+        <f>'SuperEnduro raw'!A6</f>
+        <v>Czech Republic</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Czech Republic - Prague/Tipsport Arena</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="106" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>